<commit_message>
add score calculator to excel
</commit_message>
<xml_diff>
--- a/seminar-materials/innovation-game-tool.xlsx
+++ b/seminar-materials/innovation-game-tool.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/ph8148kr_lu_se/Documents/teaching/innovation-sustainability/website/seminar-materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/research/teaching/innovation-system-game/seminar-materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD7F8013-BF4E-46A0-9BC6-DA9B64C9175F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48083326-0D45-B94B-9C9A-C655C8C74934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{56418872-B4C9-4B43-BA88-5B855C19A3CA}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D48A383F-DFFF-4A1E-B42E-2632C4DAF965}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" xr2:uid="{56418872-B4C9-4B43-BA88-5B855C19A3CA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" xr2:uid="{D48A383F-DFFF-4A1E-B42E-2632C4DAF965}"/>
   </bookViews>
   <sheets>
     <sheet name="facilitator" sheetId="1" r:id="rId1"/>
     <sheet name="participants" sheetId="2" r:id="rId2"/>
+    <sheet name="dashboard" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">facilitator!$G$2:$G$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">facilitator!$H$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">facilitator!$H$2:$H$12</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">facilitator!$I$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">facilitator!$I$2:$I$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -98,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Round</t>
   </si>
@@ -137,12 +145,60 @@
 By typing in the current round number the economy and the envrionment scores are updated automatically on their screen.
 This is great to use with the option "New Window" under the "View" tab.</t>
   </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Economic Multiplier</t>
+  </si>
+  <si>
+    <t>Calculation Helper</t>
+  </si>
+  <si>
+    <t>Four of a Kind Multiplier</t>
+  </si>
+  <si>
+    <t>Card Value</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Environmenal Innovation Count</t>
+  </si>
+  <si>
+    <t>Sum of Round:</t>
+  </si>
+  <si>
+    <t>Economic Values of Cards Played</t>
+  </si>
+  <si>
+    <t>Number of Cards for Economic Innovations</t>
+  </si>
+  <si>
+    <t>Number of Cards for Envrionmental</t>
+  </si>
+  <si>
+    <t>Economic Values of Economic Innovations</t>
+  </si>
+  <si>
+    <t>Economic Values of Environemnatl Innovation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,12 +232,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -299,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -318,6 +368,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +390,1843 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7356598529511544E-2"/>
+          <c:y val="0.12209989694039833"/>
+          <c:w val="0.93512472852057205"/>
+          <c:h val="0.86216286125595487"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>facilitator!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Environment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>facilitator!$I$2:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-381B-5240-88CC-B65787A48B2A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1639639135"/>
+        <c:axId val="714565952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1639639135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="714565952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="714565952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1639639135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>facilitator!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>The Economy TM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>facilitator!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>facilitator!$H$2:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E23-6349-A1B4-A3B8D9913780}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="715850448"/>
+        <c:axId val="715437856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="715850448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715437856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="715437856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715850448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>722756</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>16671</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>677333</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>65616</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84770F1F-EE7D-45B0-C335-1D1243526FB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>643466</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>93133</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137584</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6434F7C2-881A-CB15-9C3F-6E46ACAB20F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Philipp Jonas Kreutzer" id="{28A2558E-DFB8-4D80-BD26-93330932D423}" userId="S::ph8148kr@lu.se::b3324ed5-2aee-4d2f-8656-89595894f00c" providerId="AD"/>
@@ -342,9 +2234,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -382,7 +2274,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -488,7 +2380,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -630,7 +2522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -666,27 +2558,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6319576-2D43-4538-AC23-DB87817DD3FF}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="24.5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -712,8 +2611,32 @@
       <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="K1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -738,64 +2661,120 @@
       <c r="I2" s="7">
         <v>10</v>
       </c>
+      <c r="K2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9">
+        <f>IF(M2=4, L2*M2*$L$15, L2*M2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="9">
+        <f>IF(M2=4, L2*M2*$L$15*$L$16, L2*M2*$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>SUM(O2,P2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>IF(N2 =2, 1, IF(N2 = 4, 2, 0))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
-        <v>35</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>41</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="G3" s="7">
         <v>1</v>
       </c>
       <c r="H3" s="9">
         <f>H2-B3+C3+D3</f>
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I3" s="9">
         <f>MIN(10, I2-MAX(1,ROUND(H3/100,0))+E3)</f>
         <v>9</v>
       </c>
+      <c r="K3" s="15">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="9">
+        <f t="shared" ref="O3:O14" si="0">IF(M3=4, L3*M3*$L$15, L3*M3)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P14" si="1">IF(M3=4, L3*M3*$L$15*$L$16, L3*M3*$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q14" si="2">SUM(O3,P3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" ref="R3:R14" si="3">IF(N3 =2, 1, IF(N3 = 4, 2, 0))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
-        <v>50</v>
-      </c>
-      <c r="C4" s="8">
-        <v>80</v>
-      </c>
-      <c r="D4" s="8">
-        <v>41</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="G4" s="7">
         <v>2</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" ref="H4:H12" si="0">H3-B4+C4+D4</f>
-        <v>177</v>
+        <f t="shared" ref="H4:H12" si="4">H3-B4+C4+D4</f>
+        <v>100</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" ref="I4:I12" si="1">MIN(10, I3-MAX(1,ROUND(H4/100,0))+E4)</f>
+        <f t="shared" ref="I4:I12" si="5">MIN(10, I3-MAX(1,ROUND(H4/100,0))+E4)</f>
         <v>8</v>
       </c>
+      <c r="K4" s="15">
+        <v>3</v>
+      </c>
+      <c r="L4" s="7">
+        <v>3</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -807,15 +2786,39 @@
         <v>3</v>
       </c>
       <c r="H5" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="K5" s="15">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7">
+        <v>4</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -827,15 +2830,39 @@
         <v>4</v>
       </c>
       <c r="H6" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="K6" s="15">
+        <v>5</v>
+      </c>
+      <c r="L6" s="7">
+        <v>5</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -848,14 +2875,38 @@
       </c>
       <c r="H7" s="9">
         <f>H6-B7+C7+D7</f>
-        <v>177</v>
+        <v>100</v>
       </c>
       <c r="I7" s="9">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="K7" s="15">
+        <v>6</v>
+      </c>
+      <c r="L7" s="7">
+        <v>6</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -867,15 +2918,39 @@
         <v>6</v>
       </c>
       <c r="H8" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K8" s="15">
+        <v>7</v>
+      </c>
+      <c r="L8" s="7">
+        <v>7</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="P8" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -887,15 +2962,39 @@
         <v>7</v>
       </c>
       <c r="H9" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K9" s="15">
+        <v>8</v>
+      </c>
+      <c r="L9" s="7">
+        <v>8</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="9">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -907,15 +3006,39 @@
         <v>8</v>
       </c>
       <c r="H10" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K10" s="15">
+        <v>9</v>
+      </c>
+      <c r="L10" s="7">
+        <v>9</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -927,15 +3050,39 @@
         <v>9</v>
       </c>
       <c r="H11" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="15">
+        <v>10</v>
+      </c>
+      <c r="L11" s="7">
+        <v>10</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="P11" s="9">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -947,34 +3094,142 @@
         <v>10</v>
       </c>
       <c r="H12" s="9">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="7">
+        <v>11</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="P12" s="9">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="7">
+        <v>12</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="7">
+        <v>13</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="16">
+        <f>SUM(Q2:Q14)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="16">
+        <f>SUM(R2:R14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:P14" xr:uid="{CE3B522C-6C38-7041-A198-F6DF53F2D975}">
+      <formula1>"2,4"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -992,15 +3247,15 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="3:5" ht="40.5" x14ac:dyDescent="0.7">
+    <row r="9" spans="3:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="3:5" ht="40" x14ac:dyDescent="0.5">
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1011,17 +3266,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="3:5" ht="41" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="4">
         <v>10</v>
       </c>
       <c r="D11" s="5">
         <f>INDEX(facilitator!H2:H12,MATCH(C11, facilitator!G2:G12, 0))</f>
-        <v>177</v>
+        <v>100</v>
       </c>
       <c r="E11" s="6">
         <f>INDEX(facilitator!I2:I12,MATCH(participants!C11,facilitator!G2:G12,0))</f>
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1029,4 +3284,26 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FEB508-AEFF-7E4E-AF7F-F94B86B3CD02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>